<commit_message>
Final resubmit (without Gibbs-USBanks)W
</commit_message>
<xml_diff>
--- a/abc4sfa/4_error_measurements/data/output/simulations/exp/efficiency_metrics_abc_tun_exp_2025-04-23.xlsx
+++ b/abc4sfa/4_error_measurements/data/output/simulations/exp/efficiency_metrics_abc_tun_exp_2025-04-23.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/juanrengifo101/Documents/_OneDrive/_Publicaciones/_apolo/auto_apolo/abc4sfa/4_error_measurements/data/output/simulations/exp/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BA03E669-2AFE-A543-88F9-67F1F1D70238}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C046097B-8C1C-BA4A-8200-D86303BE4F36}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -447,7 +447,7 @@
   <dimension ref="A1:R10"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="133" workbookViewId="0">
-      <selection activeCell="O17" sqref="O17"/>
+      <selection activeCell="O20" sqref="O20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1014,11 +1014,11 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="C2:R4">
-    <cfRule type="colorScale" priority="3">
+    <cfRule type="colorScale" priority="4">
       <colorScale>
-        <cfvo type="min"/>
+        <cfvo type="formula" val="-MAX(ABS($C$2:$R$4))"/>
         <cfvo type="num" val="0"/>
-        <cfvo type="max"/>
+        <cfvo type="formula" val="MAX(ABS($C$2:$R$4))"/>
         <color rgb="FFFF0000"/>
         <color theme="0"/>
         <color rgb="FFFF0000"/>
@@ -1026,12 +1026,12 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C5:R7">
-    <cfRule type="colorScale" priority="2">
+    <cfRule type="colorScale" priority="3">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="max"/>
-        <color rgb="FFFCFCFF"/>
-        <color rgb="FF63BE7B"/>
+        <color rgb="FFFF0000"/>
+        <color theme="0"/>
       </colorScale>
     </cfRule>
   </conditionalFormatting>
@@ -1040,8 +1040,8 @@
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="max"/>
-        <color rgb="FF63BE7B"/>
-        <color rgb="FFFCFCFF"/>
+        <color theme="0"/>
+        <color rgb="FFFF0000"/>
       </colorScale>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
New Gibbs USBanks plot
</commit_message>
<xml_diff>
--- a/abc4sfa/4_error_measurements/data/output/simulations/exp/efficiency_metrics_abc_tun_exp_2025-04-23.xlsx
+++ b/abc4sfa/4_error_measurements/data/output/simulations/exp/efficiency_metrics_abc_tun_exp_2025-04-23.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/juanrengifo101/Documents/_OneDrive/_Publicaciones/_apolo/auto_apolo/abc4sfa/4_error_measurements/data/output/simulations/exp/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C046097B-8C1C-BA4A-8200-D86303BE4F36}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{658F0E86-79D2-7448-96CD-8494ACD8A451}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -447,7 +447,7 @@
   <dimension ref="A1:R10"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="133" workbookViewId="0">
-      <selection activeCell="O20" sqref="O20"/>
+      <selection activeCell="K16" sqref="K16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>

</xml_diff>